<commit_message>
added PDF and continued 2 of CC
</commit_message>
<xml_diff>
--- a/Theorie/TCPCongestionControl/TCP_Congestion_Control_Alex.xlsx
+++ b/Theorie/TCPCongestionControl/TCP_Congestion_Control_Alex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bwedu-my.sharepoint.com/personal/al_schapelt_bwedu_de/Documents/Dokumente/HTWG/Sem5/RECHNE/projects/Rechnernetze/Theorie/TCPCongestionControl/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josef\Documents\HTWG\Rechnernetze\Theorie\TCPCongestionControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E3D6F24-8E6C-449B-8B1D-6E384954ED24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF1C859-6552-4CC9-941F-F34E29751FCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aufgabe 1" sheetId="5" r:id="rId1"/>
@@ -21,12 +21,20 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="66">
   <si>
     <t>RTT</t>
   </si>
@@ -119,6 +127,111 @@
   </si>
   <si>
     <t>ack 13 -&gt; 17; ack 14 -&gt; 18, ack 15 (old CA -&gt; cwnd + 1) -&gt; 19 (new CA), 20</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>65335</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>4-9</t>
+  </si>
+  <si>
+    <t>4,8,9</t>
+  </si>
+  <si>
+    <t>3x4</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2x4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>12-13</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>10,5</t>
+  </si>
+  <si>
+    <t>3. DupACK, ssthresh=flightsize1/2 bei drittem Dup-ACK, cwnd=ssthresh + 3</t>
+  </si>
+  <si>
+    <t>2. DupACK, cwnd bleibt gleich bei erste beiden Dup-ACK, pro Dup-ACK 1 Paket losschicken</t>
+  </si>
+  <si>
+    <t>14-15</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>2x5</t>
+  </si>
+  <si>
+    <t>7,5</t>
+  </si>
+  <si>
+    <t>8,5</t>
+  </si>
+  <si>
+    <t>bei new ACK cwnd=ssthresh</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>1. DupACK</t>
+  </si>
+  <si>
+    <t>2. DupACK</t>
+  </si>
+  <si>
+    <t>4. DupACK</t>
+  </si>
+  <si>
+    <t>5,5</t>
+  </si>
+  <si>
+    <t>3. DupACK, unklar was hier gemacht werden soll, da dupACKcount == 3 aber ACK für Paket 16 ist noch gar nicht angekommen</t>
   </si>
 </sst>
 </file>
@@ -160,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -178,9 +291,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
@@ -195,8 +305,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -480,38 +606,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C4A9D5-F297-41C9-8ED9-BCC488D7955D}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="10.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="131.109375" style="7" customWidth="1"/>
+    <col min="1" max="6" width="10.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="131.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +675,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -568,7 +694,7 @@
       <c r="F3" s="1">
         <v>3</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>17</v>
       </c>
       <c r="H3" s="2">
@@ -577,17 +703,17 @@
       <c r="I3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -621,11 +747,11 @@
       <c r="K4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -660,7 +786,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>2</v>
@@ -692,11 +818,11 @@
       <c r="K6" s="4">
         <v>9</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -718,7 +844,7 @@
       </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -753,7 +879,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>9</v>
@@ -785,11 +911,11 @@
       <c r="K9" s="4">
         <v>12</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="L9" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -823,9 +949,9 @@
       <c r="K10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="9"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1">
         <v>12</v>
@@ -858,7 +984,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -892,11 +1018,11 @@
       <c r="K12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="L12" s="7" t="s">
+      <c r="L12" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -906,7 +1032,7 @@
       <c r="G13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -916,7 +1042,7 @@
       <c r="G14" s="4"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -926,7 +1052,7 @@
       <c r="G15" s="4"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -936,7 +1062,7 @@
       <c r="G16" s="4"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -946,7 +1072,7 @@
       <c r="G17" s="4"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -956,7 +1082,7 @@
       <c r="G18" s="4"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -966,7 +1092,7 @@
       <c r="G19" s="4"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -976,7 +1102,7 @@
       <c r="G20" s="4"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -986,7 +1112,7 @@
       <c r="G21" s="4"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -996,7 +1122,7 @@
       <c r="G22" s="4"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1006,7 +1132,7 @@
       <c r="G23" s="4"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1016,7 +1142,7 @@
       <c r="G24" s="4"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1026,7 +1152,7 @@
       <c r="G25" s="4"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1048,334 +1174,609 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="10.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="131.109375" style="7" customWidth="1"/>
+    <col min="1" max="6" width="10.7109375" style="13" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="13" customWidth="1"/>
+    <col min="12" max="12" width="131.140625" style="16" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="4"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="8"/>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="8"/>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="8"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="4"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="9"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="4"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="4"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="4"/>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="4"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="4"/>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="4"/>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="4"/>
-      <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="4"/>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="4"/>
-      <c r="K17" s="4"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="4"/>
-      <c r="K19" s="4"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="4"/>
-      <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="4"/>
-      <c r="K21" s="4"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="4"/>
-      <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="4"/>
-      <c r="K23" s="4"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="4"/>
-      <c r="K24" s="4"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="4"/>
-      <c r="K25" s="4"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="4"/>
-      <c r="K26" s="4"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="4"/>
-      <c r="K27" s="4"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>0</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="13">
+        <v>0</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0</v>
+      </c>
+      <c r="E3" s="13">
+        <v>65335</v>
+      </c>
+      <c r="F3" s="13">
+        <v>3</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="13">
+        <v>3</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="15">
+        <v>3</v>
+      </c>
+      <c r="K3" s="15">
+        <v>3</v>
+      </c>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>1</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="13">
+        <v>6</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="15">
+        <v>65335</v>
+      </c>
+      <c r="F5" s="13">
+        <v>7</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="13">
+        <v>7</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="15">
+        <v>65335</v>
+      </c>
+      <c r="F6" s="13">
+        <v>7</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="13">
+        <v>9</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="15">
+        <f>C7/2</f>
+        <v>4.5</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="13">
+        <v>9</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="15">
+        <f t="shared" ref="E8:E9" si="0">C8/2</f>
+        <v>4.5</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="15"/>
+      <c r="L8" s="17"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="15">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="15">
+        <v>17</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="15">
+        <v>18</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="15">
+        <v>6</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="K17" s="15"/>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="K20" s="15"/>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="K21" s="15"/>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="K22" s="15"/>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="K23" s="15"/>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="K24" s="15"/>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="K25" s="15"/>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="K26" s="15"/>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="K27" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
other solution of TCP congestion_control 2
</commit_message>
<xml_diff>
--- a/Theorie/TCPCongestionControl/TCP_Congestion_Control_Alex.xlsx
+++ b/Theorie/TCPCongestionControl/TCP_Congestion_Control_Alex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josef\Documents\HTWG\Rechnernetze\Theorie\TCPCongestionControl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bwedu-my.sharepoint.com/personal/al_schapelt_bwedu_de/Documents/Dokumente/HTWG/Sem5/RECHNE/projects/Rechnernetze/Theorie/TCPCongestionControl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF1C859-6552-4CC9-941F-F34E29751FCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{4EF1C859-6552-4CC9-941F-F34E29751FCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F428F37D-A300-4BDA-9639-200C75351D02}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-5520" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aufgabe 1" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="49">
   <si>
     <t>RTT</t>
   </si>
@@ -129,15 +129,6 @@
     <t>ack 13 -&gt; 17; ack 14 -&gt; 18, ack 15 (old CA -&gt; cwnd + 1) -&gt; 19 (new CA), 20</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>65335</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>4-9</t>
   </si>
   <si>
@@ -147,91 +138,49 @@
     <t>3x4</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>2x4</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>12-13</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>4,5</t>
-  </si>
-  <si>
-    <t>10,5</t>
-  </si>
-  <si>
     <t>3. DupACK, ssthresh=flightsize1/2 bei drittem Dup-ACK, cwnd=ssthresh + 3</t>
   </si>
   <si>
     <t>2. DupACK, cwnd bleibt gleich bei erste beiden Dup-ACK, pro Dup-ACK 1 Paket losschicken</t>
   </si>
   <si>
-    <t>14-15</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>2x5</t>
-  </si>
-  <si>
-    <t>7,5</t>
-  </si>
-  <si>
-    <t>8,5</t>
-  </si>
-  <si>
-    <t>bei new ACK cwnd=ssthresh</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>1. DupACK</t>
   </si>
   <si>
-    <t>2. DupACK</t>
-  </si>
-  <si>
-    <t>4. DupACK</t>
-  </si>
-  <si>
-    <t>5,5</t>
-  </si>
-  <si>
-    <t>3. DupACK, unklar was hier gemacht werden soll, da dupACKcount == 3 aber ACK für Paket 16 ist noch gar nicht angekommen</t>
+    <t>bei new ACK cwnd=ssthresh, ab jetzt CA phase</t>
+  </si>
+  <si>
+    <t>5-12</t>
+  </si>
+  <si>
+    <t>übertragung nach cwnd -&gt; cwnd-flightsize1 = 1.5 -&gt; 1 Segment schicken, Timer für packet 14 triggert später retransmission</t>
+  </si>
+  <si>
+    <t>12. RTT -&gt; RTO läuft ab, weiter mit slow start</t>
+  </si>
+  <si>
+    <t>neuer slow start mit cwnd=1 und ssthresh = flightsize1/2</t>
+  </si>
+  <si>
+    <t>15-25</t>
+  </si>
+  <si>
+    <t>keine acks mehr unterwegs -&gt; nächster RTO</t>
+  </si>
+  <si>
+    <t>normale slow start pahse</t>
+  </si>
+  <si>
+    <t>CA phase</t>
+  </si>
+  <si>
+    <t>nächstes paket wäre neues CA segment</t>
   </si>
 </sst>
 </file>
@@ -302,12 +251,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -323,6 +266,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -610,34 +559,34 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="10.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="131.140625" style="6" customWidth="1"/>
+    <col min="1" max="6" width="10.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="131.109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -675,7 +624,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -713,7 +662,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -751,7 +700,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -786,7 +735,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>2</v>
@@ -822,7 +771,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -844,7 +793,7 @@
       </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -879,7 +828,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>9</v>
@@ -915,7 +864,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -951,7 +900,7 @@
       </c>
       <c r="L10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1">
         <v>12</v>
@@ -984,7 +933,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -1022,7 +971,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1032,7 +981,7 @@
       <c r="G13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1042,7 +991,7 @@
       <c r="G14" s="4"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1052,7 +1001,7 @@
       <c r="G15" s="4"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1062,7 +1011,7 @@
       <c r="G16" s="4"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1072,7 +1021,7 @@
       <c r="G17" s="4"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1082,7 +1031,7 @@
       <c r="G18" s="4"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1092,7 +1041,7 @@
       <c r="G19" s="4"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1102,7 +1051,7 @@
       <c r="G20" s="4"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1112,7 +1061,7 @@
       <c r="G21" s="4"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1122,7 +1071,7 @@
       <c r="G22" s="4"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1132,7 +1081,7 @@
       <c r="G23" s="4"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1142,7 +1091,7 @@
       <c r="G24" s="4"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1152,7 +1101,7 @@
       <c r="G25" s="4"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1175,602 +1124,684 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="10.7109375" style="13" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="13" customWidth="1"/>
-    <col min="12" max="12" width="131.140625" style="16" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="12"/>
+    <col min="1" max="6" width="10.6640625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" style="11" customWidth="1"/>
+    <col min="12" max="12" width="131.109375" style="14" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
-        <v>0</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="13">
-        <v>0</v>
-      </c>
-      <c r="D3" s="13">
-        <v>0</v>
-      </c>
-      <c r="E3" s="13">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>0</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0</v>
+      </c>
+      <c r="E3" s="11">
         <v>65335</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="11">
         <v>3</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="11">
         <v>3</v>
       </c>
-      <c r="I3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="15">
+      <c r="I3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="13">
         <v>3</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K3" s="13">
         <v>3</v>
       </c>
-      <c r="L3" s="14"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="L3" s="12"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
         <v>1</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>65335</v>
+      </c>
+      <c r="F4" s="11">
+        <v>6</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="15" t="s">
+      <c r="H4" s="1">
+        <v>6</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="13">
-        <v>6</v>
-      </c>
-      <c r="G4" s="15" t="s">
+      <c r="K4" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="13">
+        <v>65335</v>
+      </c>
+      <c r="F5" s="11">
+        <v>7</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="11">
+        <v>7</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="13" t="s">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="13">
+        <v>65335</v>
+      </c>
+      <c r="F6" s="11">
+        <v>7</v>
+      </c>
+      <c r="G6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="H6" s="11">
+        <v>9</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="15">
-        <v>65335</v>
-      </c>
-      <c r="F5" s="13">
-        <v>7</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="13">
-        <v>7</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="15">
-        <v>65335</v>
-      </c>
-      <c r="F6" s="13">
-        <v>7</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="13">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
         <v>9</v>
       </c>
-      <c r="I6" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="15">
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="E7" s="13">
         <f>C7/2</f>
         <v>4.5</v>
       </c>
-      <c r="F7" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="13">
+      <c r="F7" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="G7" s="3">
+        <v>5</v>
+      </c>
+      <c r="H7" s="11">
         <v>9</v>
       </c>
-      <c r="I7" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="15">
+      <c r="I7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="1">
+        <v>5</v>
+      </c>
+      <c r="K7" s="3">
+        <v>5</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>9</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
+      <c r="E8" s="13">
         <f t="shared" ref="E8:E9" si="0">C8/2</f>
         <v>4.5</v>
       </c>
-      <c r="F8" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="15"/>
-      <c r="L8" s="17"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="15">
+      <c r="F8" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="13"/>
+      <c r="L8" s="15"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3">
+        <v>6</v>
+      </c>
+      <c r="E9" s="13">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="G9" s="3">
+        <v>14</v>
+      </c>
+      <c r="H9" s="1">
+        <v>10</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="1">
+        <v>10</v>
+      </c>
+      <c r="K9" s="3">
+        <v>5</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1">
+        <v>9</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <v>6</v>
+      </c>
+      <c r="H13" s="1">
+        <v>9</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="1">
+        <v>6</v>
+      </c>
+      <c r="K13" s="3">
+        <v>6</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>4</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>7</v>
+      </c>
+      <c r="H16" s="1">
+        <v>8</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="1">
+        <v>7</v>
+      </c>
+      <c r="K16" s="3">
+        <v>14</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>27</v>
+      </c>
+      <c r="B17" s="1">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>4</v>
+      </c>
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="1">
+        <v>2</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="L10" s="16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="15">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>28</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>4</v>
+      </c>
+      <c r="F18" s="1">
+        <v>4</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="1">
+        <v>4</v>
+      </c>
+      <c r="I18" s="1">
         <v>17</v>
       </c>
-      <c r="H11" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="L11" s="16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="15">
-        <v>18</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="L12" s="16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" s="15">
-        <v>6</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="L13" s="16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="L14" s="16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="J15" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="K15" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="K16" s="15"/>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="K17" s="15"/>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="K19" s="15"/>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="K20" s="15"/>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="K21" s="15"/>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="K22" s="15"/>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="K23" s="15"/>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="K24" s="15"/>
-    </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="K25" s="15"/>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="K26" s="15"/>
-    </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="K27" s="15"/>
+      <c r="J18" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>29</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>4</v>
+      </c>
+      <c r="F19" s="1">
+        <v>5</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="13"/>
+      <c r="L19" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="K20" s="13"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="K21" s="13"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="K22" s="13"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="K23" s="13"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="K24" s="13"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="K25" s="13"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="K26" s="13"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="K27" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
added colors to solution
</commit_message>
<xml_diff>
--- a/Theorie/TCPCongestionControl/TCP_Congestion_Control_Alex.xlsx
+++ b/Theorie/TCPCongestionControl/TCP_Congestion_Control_Alex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bwedu-my.sharepoint.com/personal/al_schapelt_bwedu_de/Documents/Dokumente/HTWG/Sem5/RECHNE/projects/Rechnernetze/Theorie/TCPCongestionControl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{4EF1C859-6552-4CC9-941F-F34E29751FCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F428F37D-A300-4BDA-9639-200C75351D02}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="13_ncr:1_{4EF1C859-6552-4CC9-941F-F34E29751FCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{05A32096-98CD-49F5-9F5A-45C466648121}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-5520" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="54">
   <si>
     <t>RTT</t>
   </si>
@@ -181,6 +181,21 @@
   </si>
   <si>
     <t>nächstes paket wäre neues CA segment</t>
+  </si>
+  <si>
+    <t>legende:</t>
+  </si>
+  <si>
+    <t>slow start</t>
+  </si>
+  <si>
+    <t>fast recovery</t>
+  </si>
+  <si>
+    <t>retransmit (entweder durch fast retransmit oder durch RTO)</t>
+  </si>
+  <si>
+    <t>congestion avoidance</t>
   </si>
 </sst>
 </file>
@@ -196,7 +211,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,11 +224,87 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -222,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -272,6 +363,51 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1121,10 +1257,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1155,7 +1291,7 @@
       <c r="K1" s="17"/>
       <c r="L1" s="17"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -1193,8 +1329,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="24">
         <v>0</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -1229,8 +1365,8 @@
       </c>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="24">
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
@@ -1265,7 +1401,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="A5" s="26">
         <v>2</v>
       </c>
       <c r="B5" s="1">
@@ -1300,6 +1436,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="27"/>
       <c r="B6" s="11" t="s">
         <v>34</v>
       </c>
@@ -1335,6 +1472,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="28"/>
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -1370,7 +1508,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="29"/>
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1394,7 +1533,7 @@
       <c r="L8" s="15"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+      <c r="A9" s="22">
         <v>3</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -1432,7 +1571,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="23"/>
       <c r="B10" s="1">
         <v>5</v>
       </c>
@@ -1459,8 +1599,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="30">
         <v>4</v>
       </c>
       <c r="B11" s="1">
@@ -1489,8 +1629,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="31" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1519,8 +1659,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="32">
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1557,8 +1697,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="25">
         <v>14</v>
       </c>
       <c r="B14" s="1">
@@ -1584,8 +1724,8 @@
       <c r="J14" s="1"/>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="24" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1614,8 +1754,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="32">
         <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1652,8 +1792,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="25">
         <v>27</v>
       </c>
       <c r="B17" s="1">
@@ -1690,8 +1830,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="25">
         <v>28</v>
       </c>
       <c r="B18" s="13" t="s">
@@ -1728,8 +1868,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="25">
         <v>29</v>
       </c>
       <c r="B19" s="13" t="s">
@@ -1802,6 +1942,31 @@
       <c r="E27" s="13"/>
       <c r="G27" s="13"/>
       <c r="K27" s="13"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L31" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L32" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L33" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L34" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L35" s="21" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>